<commit_message>
Update Excel to match modifications in bot
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador-E-Multiusuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Facturador-E-Multiusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F384827-14D4-4F27-9C8E-26971990C9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AE498-9758-4D9B-B968-7F6B11663907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tablas" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AT$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AU$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1235">
   <si>
     <t>Fecha</t>
   </si>
@@ -3739,6 +3739,9 @@
   </si>
   <si>
     <t>0003</t>
+  </si>
+  <si>
+    <t>ST</t>
   </si>
 </sst>
 </file>
@@ -4370,14 +4373,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4764,2332 +4767,2382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT17"/>
+  <dimension ref="A1:AU17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12" customWidth="1"/>
-    <col min="15" max="16" width="29" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="31" width="9.140625" customWidth="1"/>
-    <col min="32" max="32" width="13.85546875" customWidth="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" customWidth="1"/>
-    <col min="36" max="37" width="9.140625" customWidth="1"/>
-    <col min="38" max="38" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6" customWidth="1"/>
-    <col min="41" max="41" width="5.85546875" customWidth="1"/>
-    <col min="42" max="42" width="8.42578125" customWidth="1"/>
-    <col min="43" max="43" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12" customWidth="1"/>
+    <col min="21" max="22" width="29" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="37" width="9.140625" customWidth="1"/>
+    <col min="38" max="38" width="13.85546875" customWidth="1"/>
+    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6" customWidth="1"/>
+    <col min="45" max="45" width="5.85546875" customWidth="1"/>
+    <col min="46" max="46" width="8.42578125" customWidth="1"/>
+    <col min="47" max="47" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:47" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1231</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>1229</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>1228</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>1227</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>1208</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>1209</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>1210</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>1211</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="X1" s="16" t="s">
         <v>1212</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="AA1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="AC1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="AE1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="AF1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AG1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AH1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AI1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AJ1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AE1" s="16" t="s">
+      <c r="AK1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AL1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AM1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AN1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AO1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>1230</v>
-      </c>
-      <c r="AL1" s="16" t="s">
+      <c r="AP1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="AM1" s="16" t="s">
+      <c r="AQ1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AR1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="AO1" s="17" t="s">
+      <c r="AS1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AP1" s="17" t="s">
+      <c r="AT1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="AQ1" s="17" t="s">
+      <c r="AU1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AR1" s="17" t="s">
-        <v>1224</v>
-      </c>
-      <c r="AS1" s="17" t="s">
-        <v>1225</v>
-      </c>
-      <c r="AT1" s="17" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="7">
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="7">
         <f ca="1">TODAY()</f>
-        <v>45143</v>
-      </c>
-      <c r="C2" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="M2" s="23">
-        <f>IFERROR(VLOOKUP(L2,CUIT_paises[],2,0),"")</f>
-        <v>55000002126</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="S2" s="23">
+        <f>IFERROR(VLOOKUP(R2,CUIT_paises[],2,0),"")</f>
+        <v>55000002126</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="4">
+      <c r="Z2" s="4">
         <v>7.003044</v>
       </c>
-      <c r="U2" s="5">
+      <c r="AA2" s="5">
         <v>19000</v>
       </c>
-      <c r="V2" s="5">
-        <f>T2*U2</f>
+      <c r="AB2" s="5">
+        <f>Z2*AA2</f>
         <v>133057.83600000001</v>
       </c>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="13">
-        <f>COUNTIFS($D$1:D2,D2,$O$1:O2,O2)+1</f>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="13">
+        <f>COUNTIFS($J$1:J2,J2,$U$1:U2,U2)+1</f>
         <v>2</v>
       </c>
-      <c r="AB2" s="15" t="str">
-        <f>SUBSTITUTE(T2,",",".")</f>
+      <c r="AH2" s="15" t="str">
+        <f>SUBSTITUTE(Z2,",",".")</f>
         <v>7.003044</v>
       </c>
-      <c r="AC2" s="15" t="str">
-        <f t="shared" ref="AC2:AC17" si="0">SUBSTITUTE(TEXT(U2,"0,00"),",",".")</f>
+      <c r="AI2" s="15" t="str">
+        <f t="shared" ref="AI2:AI17" si="0">SUBSTITUTE(TEXT(AA2,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
-      <c r="AD2" s="1" t="str">
-        <f t="shared" ref="AD2:AD17" si="1">TEXT(X2,"00000")</f>
+      <c r="AJ2" s="1" t="str">
+        <f t="shared" ref="AJ2:AJ17" si="1">TEXT(AD2,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="AE2" s="1" t="str">
-        <f t="shared" ref="AE2:AE17" si="2">TEXT(Y2,"00000000")</f>
+      <c r="AK2" s="1" t="str">
+        <f t="shared" ref="AK2:AK17" si="2">TEXT(AE2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="AF2" s="8">
-        <f>Z2</f>
+      <c r="AL2" s="8">
+        <f>AF2</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="12">
-        <f>IF(AP2="A",ROUND(V2+#REF!,2),ROUND(V2,2))</f>
+      <c r="AM2" s="12">
+        <f>IF(AT2="A",ROUND(AB2+#REF!,2),ROUND(AB2,2))</f>
         <v>133057.84</v>
       </c>
-      <c r="AH2" s="9" t="str">
-        <f t="shared" ref="AH2:AH17" si="3">IF(RIGHT(D2,1)="A",SUBSTITUTE(TEXT(V2,"0,00"),",","."),SUBSTITUTE(TEXT(AG2,"0,00"),",","."))</f>
+      <c r="AN2" s="9" t="str">
+        <f t="shared" ref="AN2:AN17" si="3">IF(RIGHT(J2,1)="A",SUBSTITUTE(TEXT(AB2,"0,00"),",","."),SUBSTITUTE(TEXT(AM2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
-      <c r="AI2" s="9" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AG2,0)-AG2,"0,00"),",",".")</f>
+      <c r="AO2" s="9" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AM2,0)-AM2,"0,00"),",",".")</f>
         <v>0.16</v>
       </c>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="1">
-        <f t="shared" ref="AL2:AL17" si="4">ROW(O2)</f>
+      <c r="AP2" s="1">
+        <f t="shared" ref="AP2:AP17" si="4">ROW(U2)</f>
         <v>2</v>
       </c>
-      <c r="AM2" s="14" t="str">
-        <f>L2&amp;"-"&amp;COUNTIF($L$1:L2,L2)</f>
+      <c r="AQ2" s="14" t="str">
+        <f>R2&amp;"-"&amp;COUNTIF($R$1:R2,R2)</f>
         <v>ESTADOS UNIDOS - Persona Jurídica-1</v>
       </c>
-      <c r="AN2" s="1">
-        <f t="shared" ref="AN2:AN17" si="5">IF(O1=O2,1,0)</f>
+      <c r="AR2" s="1">
+        <f t="shared" ref="AR2:AR17" si="5">IF(U1=U2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AO2" s="1">
-        <f t="shared" ref="AO2:AO17" si="6">IF(O2=O3,1,0)</f>
+      <c r="AS2" s="1">
+        <f t="shared" ref="AS2:AS17" si="6">IF(U2=U3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AP2" s="1" t="str">
-        <f t="shared" ref="AP2:AP17" si="7">RIGHT(D2)</f>
+      <c r="AT2" s="1" t="str">
+        <f t="shared" ref="AT2:AT17" si="7">RIGHT(J2)</f>
         <v>E</v>
       </c>
-      <c r="AQ2" s="1">
-        <f t="shared" ref="AQ2:AQ17" si="8">IF(LEFT(D2,4)="Nota",0,1)</f>
+      <c r="AU2" s="1">
+        <f t="shared" ref="AU2:AU17" si="8">IF(LEFT(J2,4)="Nota",0,1)</f>
         <v>1</v>
       </c>
-      <c r="AR2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H17" ca="1" si="9">TODAY()</f>
+        <v>45200</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="7">
-        <f t="shared" ref="B3:B17" ca="1" si="9">TODAY()</f>
-        <v>45143</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M3" s="23">
-        <f>IFERROR(VLOOKUP(L3,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S3" s="23">
+        <f>IFERROR(VLOOKUP(R3,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2" t="s">
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S3" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T3" s="4">
+      <c r="Y3" s="1" t="str">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(H3,"mmmm"))</f>
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z3" s="4">
         <v>8.0252280000000003</v>
       </c>
-      <c r="U3" s="5">
+      <c r="AA3" s="5">
         <v>19000</v>
       </c>
-      <c r="V3" s="5">
-        <f t="shared" ref="V3:V17" si="10">T3*U3</f>
+      <c r="AB3" s="5">
+        <f t="shared" ref="AB3:AB17" si="10">Z3*AA3</f>
         <v>152479.33199999999</v>
       </c>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="13">
-        <f>COUNTIFS($D$1:D3,D3,$O$1:O3,O3)+1</f>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="13">
+        <f>COUNTIFS($J$1:J3,J3,$U$1:U3,U3)+1</f>
         <v>2</v>
       </c>
-      <c r="AB3" s="15" t="str">
-        <f t="shared" ref="AB3:AB17" si="11">SUBSTITUTE(T3,",",".")</f>
+      <c r="AH3" s="15" t="str">
+        <f t="shared" ref="AH3:AH17" si="11">SUBSTITUTE(Z3,",",".")</f>
         <v>8.025228</v>
       </c>
-      <c r="AC3" s="15" t="str">
+      <c r="AI3" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD3" s="1" t="str">
+      <c r="AJ3" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE3" s="1" t="str">
+      <c r="AK3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF3" s="8">
-        <f t="shared" ref="AF3:AF17" si="12">Z3</f>
+      <c r="AL3" s="8">
+        <f t="shared" ref="AL3:AL17" si="12">AF3</f>
         <v>0</v>
       </c>
-      <c r="AG3" s="12">
-        <f>IF(AP3="A",ROUND(V3+#REF!,2),ROUND(V3,2))</f>
+      <c r="AM3" s="12">
+        <f>IF(AT3="A",ROUND(AB3+#REF!,2),ROUND(AB3,2))</f>
         <v>152479.32999999999</v>
       </c>
-      <c r="AH3" s="9" t="str">
+      <c r="AN3" s="9" t="str">
         <f t="shared" si="3"/>
         <v>152479.33</v>
       </c>
-      <c r="AI3" s="9" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AG3,0)-AG3,"0,00"),",",".")</f>
+      <c r="AO3" s="9" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AM3,0)-AM3,"0,00"),",",".")</f>
         <v>0.67</v>
       </c>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="1">
+      <c r="AP3" s="1">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="AM3" s="14" t="str">
-        <f>L3&amp;"-"&amp;COUNTIF($L$1:L3,L3)</f>
+      <c r="AQ3" s="14" t="str">
+        <f>R3&amp;"-"&amp;COUNTIF($R$1:R3,R3)</f>
         <v>ESTADOS UNIDOS - Persona Física-1</v>
       </c>
-      <c r="AN3" s="1">
+      <c r="AR3" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO3" s="1">
+      <c r="AS3" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP3" s="1" t="str">
+      <c r="AT3" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ3" s="1">
+      <c r="AU3" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AR3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>1226</v>
       </c>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="7">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C4" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I4" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="M4" s="23">
-        <f>IFERROR(VLOOKUP(L4,CUIT_paises[],2,0),"")</f>
-        <v>51600002124</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="S4" s="23">
+        <f>IFERROR(VLOOKUP(R4,CUIT_paises[],2,0),"")</f>
+        <v>51600002124</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T4" s="4">
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="1" t="str">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(H4,"mmmm"))</f>
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z4" s="4">
         <v>10.004348999999999</v>
       </c>
-      <c r="U4" s="5">
+      <c r="AA4" s="5">
         <v>19000</v>
       </c>
-      <c r="V4" s="5">
+      <c r="AB4" s="5">
         <f t="shared" si="10"/>
         <v>190082.63099999999</v>
       </c>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="13">
-        <f>COUNTIFS($D$1:D4,D4,$O$1:O4,O4)+1</f>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="13">
+        <f>COUNTIFS($J$1:J4,J4,$U$1:U4,U4)+1</f>
         <v>2</v>
       </c>
-      <c r="AB4" s="15" t="str">
+      <c r="AH4" s="15" t="str">
         <f t="shared" si="11"/>
         <v>10.004349</v>
       </c>
-      <c r="AC4" s="15" t="str">
+      <c r="AI4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD4" s="1" t="str">
+      <c r="AJ4" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE4" s="1" t="str">
+      <c r="AK4" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF4" s="8">
+      <c r="AL4" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG4" s="12">
-        <f>IF(AP4="A",ROUND(V4+#REF!,2),ROUND(V4,2))</f>
+      <c r="AM4" s="12">
+        <f>IF(AT4="A",ROUND(AB4+#REF!,2),ROUND(AB4,2))</f>
         <v>190082.63</v>
       </c>
-      <c r="AH4" s="9" t="str">
+      <c r="AN4" s="9" t="str">
         <f t="shared" si="3"/>
         <v>190082.63</v>
       </c>
-      <c r="AI4" s="9" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AG4,0)-AG4,"0,00"),",",".")</f>
+      <c r="AO4" s="9" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AM4,0)-AM4,"0,00"),",",".")</f>
         <v>0.37</v>
       </c>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="1">
+      <c r="AP4" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AM4" s="14" t="str">
-        <f>L4&amp;"-"&amp;COUNTIF($L$1:L4,L4)</f>
+      <c r="AQ4" s="14" t="str">
+        <f>R4&amp;"-"&amp;COUNTIF($R$1:R4,R4)</f>
         <v>ESTADOS UNIDOS - Otro tipo de Entidad-1</v>
       </c>
-      <c r="AN4" s="1">
+      <c r="AR4" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO4" s="1">
+      <c r="AS4" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP4" s="1" t="str">
+      <c r="AT4" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ4" s="1">
+      <c r="AU4" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AR4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS4" s="2"/>
-      <c r="AT4" s="2"/>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="7">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C5" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="M5" s="23">
-        <f>IFERROR(VLOOKUP(L5,CUIT_paises[],2,0),"")</f>
-        <v>55000002126</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="S5" s="23">
+        <f>IFERROR(VLOOKUP(R5,CUIT_paises[],2,0),"")</f>
+        <v>55000002126</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T5" s="4">
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="1" t="str">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(H5,"mmmm"))</f>
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z5" s="4">
         <v>9.0256629999999998</v>
       </c>
-      <c r="U5" s="5">
+      <c r="AA5" s="5">
         <v>19000</v>
       </c>
-      <c r="V5" s="5">
+      <c r="AB5" s="5">
         <f t="shared" si="10"/>
         <v>171487.59700000001</v>
       </c>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="13">
-        <f>COUNTIFS($D$1:D5,D5,$O$1:O5,O5)+1</f>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="13">
+        <f>COUNTIFS($J$1:J5,J5,$U$1:U5,U5)+1</f>
         <v>2</v>
       </c>
-      <c r="AB5" s="15" t="str">
+      <c r="AH5" s="15" t="str">
         <f t="shared" si="11"/>
         <v>9.025663</v>
       </c>
-      <c r="AC5" s="15" t="str">
+      <c r="AI5" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD5" s="1" t="str">
+      <c r="AJ5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE5" s="1" t="str">
+      <c r="AK5" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF5" s="8">
+      <c r="AL5" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG5" s="12">
-        <f>IF(AP5="A",ROUND(V5+#REF!,2),ROUND(V5,2))</f>
+      <c r="AM5" s="12">
+        <f>IF(AT5="A",ROUND(AB5+#REF!,2),ROUND(AB5,2))</f>
         <v>171487.6</v>
       </c>
-      <c r="AH5" s="9" t="str">
+      <c r="AN5" s="9" t="str">
         <f t="shared" si="3"/>
         <v>171487.60</v>
       </c>
-      <c r="AI5" s="9" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AG5,0)-AG5,"0,00"),",",".")</f>
+      <c r="AO5" s="9" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AM5,0)-AM5,"0,00"),",",".")</f>
         <v>0.40</v>
       </c>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="1">
+      <c r="AP5" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="AM5" s="14" t="str">
-        <f>L5&amp;"-"&amp;COUNTIF($L$1:L5,L5)</f>
+      <c r="AQ5" s="14" t="str">
+        <f>R5&amp;"-"&amp;COUNTIF($R$1:R5,R5)</f>
         <v>ESTADOS UNIDOS - Persona Jurídica-2</v>
       </c>
-      <c r="AN5" s="1">
+      <c r="AR5" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO5" s="1">
+      <c r="AS5" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP5" s="1" t="str">
+      <c r="AT5" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ5" s="1">
+      <c r="AU5" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS5" s="2"/>
-      <c r="AT5" s="2"/>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="7">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C6" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M6" s="23">
-        <f>IFERROR(VLOOKUP(L6,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S6" s="23">
+        <f>IFERROR(VLOOKUP(R6,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T6" s="4">
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="1" t="str">
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(H6,"mmmm"))</f>
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z6" s="4">
         <v>5.0239229999999999</v>
       </c>
-      <c r="U6" s="5">
+      <c r="AA6" s="5">
         <v>19000</v>
       </c>
-      <c r="V6" s="5">
+      <c r="AB6" s="5">
         <f t="shared" si="10"/>
         <v>95454.536999999997</v>
       </c>
-      <c r="W6" s="10" t="s">
+      <c r="AC6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="X6" s="10" t="s">
+      <c r="AD6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" s="10" t="s">
+      <c r="AE6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="AF6" s="11">
         <v>44816</v>
       </c>
-      <c r="AA6" s="13">
-        <f>COUNTIFS($D$1:D6,D6,$O$1:O6,O6)+1</f>
+      <c r="AG6" s="13">
+        <f>COUNTIFS($J$1:J6,J6,$U$1:U6,U6)+1</f>
         <v>2</v>
       </c>
-      <c r="AB6" s="15" t="str">
+      <c r="AH6" s="15" t="str">
         <f t="shared" si="11"/>
         <v>5.023923</v>
       </c>
-      <c r="AC6" s="15" t="str">
+      <c r="AI6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD6" s="1" t="str">
+      <c r="AJ6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="AE6" s="1" t="str">
+      <c r="AK6" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000003</v>
       </c>
-      <c r="AF6" s="8">
+      <c r="AL6" s="8">
         <f t="shared" si="12"/>
         <v>44816</v>
       </c>
-      <c r="AG6" s="12">
-        <f>IF(AP6="A",ROUND(V6+#REF!,2),ROUND(V6,2))</f>
+      <c r="AM6" s="12">
+        <f>IF(AT6="A",ROUND(AB6+#REF!,2),ROUND(AB6,2))</f>
         <v>95454.54</v>
       </c>
-      <c r="AH6" s="9" t="str">
+      <c r="AN6" s="9" t="str">
         <f t="shared" si="3"/>
         <v>95454.54</v>
       </c>
-      <c r="AI6" s="9" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AG6,0)-AG6,"0,00"),",",".")</f>
+      <c r="AO6" s="9" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AM6,0)-AM6,"0,00"),",",".")</f>
         <v>0.46</v>
       </c>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="1">
+      <c r="AP6" s="1">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="AM6" s="14" t="str">
-        <f>L6&amp;"-"&amp;COUNTIF($L$1:L6,L6)</f>
+      <c r="AQ6" s="14" t="str">
+        <f>R6&amp;"-"&amp;COUNTIF($R$1:R6,R6)</f>
         <v>ESTADOS UNIDOS - Persona Física-2</v>
       </c>
-      <c r="AN6" s="1">
+      <c r="AR6" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO6" s="1">
+      <c r="AS6" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AP6" s="1" t="str">
+      <c r="AT6" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ6" s="1">
+      <c r="AU6" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS6" s="2"/>
-      <c r="AT6" s="2"/>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C7" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I7" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M7" s="23">
-        <f>IFERROR(VLOOKUP(L7,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S7" s="23">
+        <f>IFERROR(VLOOKUP(R7,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2" t="s">
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="Y7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="4">
+      <c r="Z7" s="4">
         <v>5.0021740000000001</v>
       </c>
-      <c r="U7" s="5">
+      <c r="AA7" s="5">
         <v>19000</v>
       </c>
-      <c r="V7" s="5">
+      <c r="AB7" s="5">
         <f t="shared" si="10"/>
         <v>95041.305999999997</v>
       </c>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="13">
-        <f>COUNTIFS($D$1:D7,D7,$O$1:O7,O7)+1</f>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="13">
+        <f>COUNTIFS($J$1:J7,J7,$U$1:U7,U7)+1</f>
         <v>3</v>
       </c>
-      <c r="AB7" s="15" t="str">
+      <c r="AH7" s="15" t="str">
         <f t="shared" si="11"/>
         <v>5.002174</v>
       </c>
-      <c r="AC7" s="15" t="str">
+      <c r="AI7" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD7" s="1" t="str">
+      <c r="AJ7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE7" s="1" t="str">
+      <c r="AK7" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF7" s="8">
+      <c r="AL7" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="12">
-        <f>IF(AP7="A",ROUND(V7+#REF!,2),ROUND(V7,2))</f>
+      <c r="AM7" s="12">
+        <f>IF(AT7="A",ROUND(AB7+#REF!,2),ROUND(AB7,2))</f>
         <v>95041.31</v>
       </c>
-      <c r="AH7" s="9" t="str">
+      <c r="AN7" s="9" t="str">
         <f t="shared" si="3"/>
         <v>95041.31</v>
       </c>
-      <c r="AI7" s="9" t="str">
-        <f t="shared" ref="AI7:AI17" si="13">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
+      <c r="AO7" s="9" t="str">
+        <f t="shared" ref="AO7:AO17" si="13">SUBSTITUTE(TEXT(ROUNDUP(AM7,0)-AM7,"0,00"),",",".")</f>
         <v>0.69</v>
       </c>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="1">
+      <c r="AP7" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="AM7" s="14" t="str">
-        <f>L7&amp;"-"&amp;COUNTIF($L$1:L7,L7)</f>
+      <c r="AQ7" s="14" t="str">
+        <f>R7&amp;"-"&amp;COUNTIF($R$1:R7,R7)</f>
         <v>ESTADOS UNIDOS - Persona Física-3</v>
       </c>
-      <c r="AN7" s="1">
+      <c r="AR7" s="1">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AO7" s="1">
+      <c r="AS7" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP7" s="1" t="str">
+      <c r="AT7" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ7" s="1">
+      <c r="AU7" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS7" s="2"/>
-      <c r="AT7" s="2"/>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="7">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C8" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I8" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M8" s="23">
-        <f>IFERROR(VLOOKUP(L8,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S8" s="23">
+        <f>IFERROR(VLOOKUP(R8,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2" t="s">
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S8" s="1" t="str">
-        <f t="shared" ref="S8:S13" ca="1" si="14">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T8" s="4">
+      <c r="Y8" s="1" t="str">
+        <f t="shared" ref="Y8:Y13" ca="1" si="14">"Honorarios "&amp;PROPER(TEXT(H8,"mmmm"))</f>
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z8" s="4">
         <v>10.004348999999999</v>
       </c>
-      <c r="U8" s="5">
+      <c r="AA8" s="5">
         <v>19000</v>
       </c>
-      <c r="V8" s="5">
+      <c r="AB8" s="5">
         <f t="shared" si="10"/>
         <v>190082.63099999999</v>
       </c>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="13">
-        <f>COUNTIFS($D$1:D8,D8,$O$1:O8,O8)+1</f>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="13">
+        <f>COUNTIFS($J$1:J8,J8,$U$1:U8,U8)+1</f>
         <v>2</v>
       </c>
-      <c r="AB8" s="15" t="str">
+      <c r="AH8" s="15" t="str">
         <f t="shared" si="11"/>
         <v>10.004349</v>
       </c>
-      <c r="AC8" s="15" t="str">
+      <c r="AI8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD8" s="1" t="str">
+      <c r="AJ8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE8" s="1" t="str">
+      <c r="AK8" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF8" s="8">
+      <c r="AL8" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG8" s="12">
-        <f>IF(AP8="A",ROUND(V8+#REF!,2),ROUND(V8,2))</f>
+      <c r="AM8" s="12">
+        <f>IF(AT8="A",ROUND(AB8+#REF!,2),ROUND(AB8,2))</f>
         <v>190082.63</v>
       </c>
-      <c r="AH8" s="9" t="str">
+      <c r="AN8" s="9" t="str">
         <f t="shared" si="3"/>
         <v>190082.63</v>
       </c>
-      <c r="AI8" s="9" t="str">
+      <c r="AO8" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.37</v>
       </c>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="1">
+      <c r="AP8" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AM8" s="14" t="str">
-        <f>L8&amp;"-"&amp;COUNTIF($L$1:L8,L8)</f>
+      <c r="AQ8" s="14" t="str">
+        <f>R8&amp;"-"&amp;COUNTIF($R$1:R8,R8)</f>
         <v>ESTADOS UNIDOS - Persona Física-4</v>
       </c>
-      <c r="AN8" s="1">
+      <c r="AR8" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO8" s="1">
+      <c r="AS8" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP8" s="1" t="str">
+      <c r="AT8" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ8" s="1">
+      <c r="AU8" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS8" s="2"/>
-      <c r="AT8" s="2"/>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="7">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C9" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M9" s="23">
-        <f>IFERROR(VLOOKUP(L9,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S9" s="23">
+        <f>IFERROR(VLOOKUP(R9,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2" t="s">
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S9" s="1" t="str">
+      <c r="Y9" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T9" s="4">
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z9" s="4">
         <v>1.0221830000000001</v>
       </c>
-      <c r="U9" s="5">
+      <c r="AA9" s="5">
         <v>19000</v>
       </c>
-      <c r="V9" s="5">
+      <c r="AB9" s="5">
         <f t="shared" si="10"/>
         <v>19421.477000000003</v>
       </c>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="13">
-        <f>COUNTIFS($D$1:D9,D9,$O$1:O9,O9)+1</f>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="13">
+        <f>COUNTIFS($J$1:J9,J9,$U$1:U9,U9)+1</f>
         <v>2</v>
       </c>
-      <c r="AB9" s="15" t="str">
+      <c r="AH9" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.022183</v>
       </c>
-      <c r="AC9" s="15" t="str">
+      <c r="AI9" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD9" s="1" t="str">
+      <c r="AJ9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE9" s="1" t="str">
+      <c r="AK9" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF9" s="8">
+      <c r="AL9" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="12">
-        <f>IF(AP9="A",ROUND(V9+#REF!,2),ROUND(V9,2))</f>
+      <c r="AM9" s="12">
+        <f>IF(AT9="A",ROUND(AB9+#REF!,2),ROUND(AB9,2))</f>
         <v>19421.48</v>
       </c>
-      <c r="AH9" s="9" t="str">
+      <c r="AN9" s="9" t="str">
         <f t="shared" si="3"/>
         <v>19421.48</v>
       </c>
-      <c r="AI9" s="9" t="str">
+      <c r="AO9" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="1">
+      <c r="AP9" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="AM9" s="14" t="str">
-        <f>L9&amp;"-"&amp;COUNTIF($L$1:L9,L9)</f>
+      <c r="AQ9" s="14" t="str">
+        <f>R9&amp;"-"&amp;COUNTIF($R$1:R9,R9)</f>
         <v>ESTADOS UNIDOS - Persona Física-5</v>
       </c>
-      <c r="AN9" s="1">
+      <c r="AR9" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO9" s="1">
+      <c r="AS9" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP9" s="1" t="str">
+      <c r="AT9" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ9" s="1">
+      <c r="AU9" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="7">
+        <f t="shared" ca="1" si="9"/>
+        <v>45200</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="7">
-        <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M10" s="23">
-        <f>IFERROR(VLOOKUP(L10,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S10" s="23">
+        <f>IFERROR(VLOOKUP(R10,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2" t="s">
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S10" s="1" t="str">
+      <c r="Y10" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T10" s="4">
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z10" s="4">
         <v>1.0439320000000001</v>
       </c>
-      <c r="U10" s="5">
+      <c r="AA10" s="5">
         <v>19000</v>
       </c>
-      <c r="V10" s="5">
+      <c r="AB10" s="5">
         <f t="shared" si="10"/>
         <v>19834.708000000002</v>
       </c>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="13">
-        <f>COUNTIFS($D$1:D10,D10,$O$1:O10,O10)+1</f>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="13">
+        <f>COUNTIFS($J$1:J10,J10,$U$1:U10,U10)+1</f>
         <v>2</v>
       </c>
-      <c r="AB10" s="15" t="str">
+      <c r="AH10" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.043932</v>
       </c>
-      <c r="AC10" s="15" t="str">
+      <c r="AI10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD10" s="1" t="str">
+      <c r="AJ10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE10" s="1" t="str">
+      <c r="AK10" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF10" s="8">
+      <c r="AL10" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG10" s="12">
-        <f>IF(AP10="A",ROUND(V10+#REF!,2),ROUND(V10,2))</f>
+      <c r="AM10" s="12">
+        <f>IF(AT10="A",ROUND(AB10+#REF!,2),ROUND(AB10,2))</f>
         <v>19834.71</v>
       </c>
-      <c r="AH10" s="9" t="str">
+      <c r="AN10" s="9" t="str">
         <f t="shared" si="3"/>
         <v>19834.71</v>
       </c>
-      <c r="AI10" s="9" t="str">
+      <c r="AO10" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.29</v>
       </c>
-      <c r="AJ10" s="2"/>
-      <c r="AK10" s="2"/>
-      <c r="AL10" s="1">
+      <c r="AP10" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="AM10" s="14" t="str">
-        <f>L10&amp;"-"&amp;COUNTIF($L$1:L10,L10)</f>
+      <c r="AQ10" s="14" t="str">
+        <f>R10&amp;"-"&amp;COUNTIF($R$1:R10,R10)</f>
         <v>ESTADOS UNIDOS - Persona Física-6</v>
       </c>
-      <c r="AN10" s="1">
+      <c r="AR10" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO10" s="1">
+      <c r="AS10" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AP10" s="1" t="str">
+      <c r="AT10" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ10" s="1">
+      <c r="AU10" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>1226</v>
       </c>
-      <c r="AS10" s="2"/>
-      <c r="AT10" s="2"/>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="7">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C11" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I11" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M11" s="23">
-        <f>IFERROR(VLOOKUP(L11,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S11" s="23">
+        <f>IFERROR(VLOOKUP(R11,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2" t="s">
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S11" s="1" t="str">
+      <c r="Y11" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T11" s="4">
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z11" s="4">
         <v>1.3</v>
       </c>
-      <c r="U11" s="5">
+      <c r="AA11" s="5">
         <v>10000</v>
       </c>
-      <c r="V11" s="5">
+      <c r="AB11" s="5">
         <f t="shared" si="10"/>
         <v>13000</v>
       </c>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="13">
-        <f>COUNTIFS($D$1:D11,D11,$O$1:O11,O11)+1</f>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="13">
+        <f>COUNTIFS($J$1:J11,J11,$U$1:U11,U11)+1</f>
         <v>3</v>
       </c>
-      <c r="AB11" s="15" t="str">
+      <c r="AH11" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.3</v>
       </c>
-      <c r="AC11" s="15" t="str">
+      <c r="AI11" s="15" t="str">
         <f t="shared" si="0"/>
         <v>10000.00</v>
       </c>
-      <c r="AD11" s="1" t="str">
+      <c r="AJ11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE11" s="1" t="str">
+      <c r="AK11" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF11" s="8">
+      <c r="AL11" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG11" s="12">
-        <f>IF(AP11="A",ROUND(V11+#REF!,2),ROUND(V11,2))</f>
+      <c r="AM11" s="12">
+        <f>IF(AT11="A",ROUND(AB11+#REF!,2),ROUND(AB11,2))</f>
         <v>13000</v>
       </c>
-      <c r="AH11" s="9" t="str">
+      <c r="AN11" s="9" t="str">
         <f t="shared" si="3"/>
         <v>13000.00</v>
       </c>
-      <c r="AI11" s="9" t="str">
+      <c r="AO11" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.00</v>
       </c>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="1">
+      <c r="AP11" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="AM11" s="14" t="str">
-        <f>L11&amp;"-"&amp;COUNTIF($L$1:L11,L11)</f>
+      <c r="AQ11" s="14" t="str">
+        <f>R11&amp;"-"&amp;COUNTIF($R$1:R11,R11)</f>
         <v>ESTADOS UNIDOS - Persona Física-7</v>
       </c>
-      <c r="AN11" s="1">
+      <c r="AR11" s="1">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AO11" s="1">
+      <c r="AS11" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP11" s="1" t="str">
+      <c r="AT11" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ11" s="1">
+      <c r="AU11" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>1226</v>
       </c>
-      <c r="AS11" s="2"/>
-      <c r="AT11" s="2"/>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="7">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C12" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I12" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M12" s="23">
-        <f>IFERROR(VLOOKUP(L12,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S12" s="23">
+        <f>IFERROR(VLOOKUP(R12,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2" t="s">
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S12" s="1" t="str">
+      <c r="Y12" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T12" s="4">
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z12" s="4">
         <v>1.2105263157894737</v>
       </c>
-      <c r="U12" s="5">
+      <c r="AA12" s="5">
         <v>19000</v>
       </c>
-      <c r="V12" s="5">
+      <c r="AB12" s="5">
         <f t="shared" si="10"/>
         <v>23000</v>
       </c>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="13">
-        <f>COUNTIFS($D$1:D12,D12,$O$1:O12,O12)+1</f>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="13">
+        <f>COUNTIFS($J$1:J12,J12,$U$1:U12,U12)+1</f>
         <v>2</v>
       </c>
-      <c r="AB12" s="15" t="str">
+      <c r="AH12" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.21052631578947</v>
       </c>
-      <c r="AC12" s="15" t="str">
+      <c r="AI12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD12" s="1" t="str">
+      <c r="AJ12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE12" s="1" t="str">
+      <c r="AK12" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF12" s="8">
+      <c r="AL12" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG12" s="12">
-        <f>IF(AP12="A",ROUND(V12+#REF!,2),ROUND(V12,2))</f>
+      <c r="AM12" s="12">
+        <f>IF(AT12="A",ROUND(AB12+#REF!,2),ROUND(AB12,2))</f>
         <v>23000</v>
       </c>
-      <c r="AH12" s="9" t="str">
+      <c r="AN12" s="9" t="str">
         <f t="shared" si="3"/>
         <v>23000.00</v>
       </c>
-      <c r="AI12" s="9" t="str">
+      <c r="AO12" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.00</v>
       </c>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="1">
+      <c r="AP12" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="AM12" s="14" t="str">
-        <f>L12&amp;"-"&amp;COUNTIF($L$1:L12,L12)</f>
+      <c r="AQ12" s="14" t="str">
+        <f>R12&amp;"-"&amp;COUNTIF($R$1:R12,R12)</f>
         <v>ESTADOS UNIDOS - Persona Física-8</v>
       </c>
-      <c r="AN12" s="1">
+      <c r="AR12" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO12" s="1">
+      <c r="AS12" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP12" s="1" t="str">
+      <c r="AT12" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ12" s="1">
+      <c r="AU12" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS12" s="2"/>
-      <c r="AT12" s="2"/>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="7">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C13" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M13" s="23">
-        <f>IFERROR(VLOOKUP(L13,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S13" s="23">
+        <f>IFERROR(VLOOKUP(R13,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2" t="s">
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S13" s="1" t="str">
+      <c r="Y13" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Honorarios Agosto</v>
-      </c>
-      <c r="T13" s="4">
+        <v>Honorarios Octubre</v>
+      </c>
+      <c r="Z13" s="4">
         <v>1.5</v>
       </c>
-      <c r="U13" s="5">
+      <c r="AA13" s="5">
         <v>19000</v>
       </c>
-      <c r="V13" s="5">
+      <c r="AB13" s="5">
         <f t="shared" si="10"/>
         <v>28500</v>
       </c>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="13">
-        <f>COUNTIFS($D$1:D13,D13,$O$1:O13,O13)+1</f>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="13">
+        <f>COUNTIFS($J$1:J13,J13,$U$1:U13,U13)+1</f>
         <v>2</v>
       </c>
-      <c r="AB13" s="15" t="str">
+      <c r="AH13" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
-      <c r="AC13" s="15" t="str">
+      <c r="AI13" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD13" s="1" t="str">
+      <c r="AJ13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00000</v>
       </c>
-      <c r="AE13" s="1" t="str">
+      <c r="AK13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
-      <c r="AF13" s="8">
+      <c r="AL13" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG13" s="12">
-        <f>IF(AP13="A",ROUND(V13+#REF!,2),ROUND(V13,2))</f>
+      <c r="AM13" s="12">
+        <f>IF(AT13="A",ROUND(AB13+#REF!,2),ROUND(AB13,2))</f>
         <v>28500</v>
       </c>
-      <c r="AH13" s="9" t="str">
+      <c r="AN13" s="9" t="str">
         <f t="shared" si="3"/>
         <v>28500.00</v>
       </c>
-      <c r="AI13" s="9" t="str">
+      <c r="AO13" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.00</v>
       </c>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="1">
+      <c r="AP13" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="AM13" s="14" t="str">
-        <f>L13&amp;"-"&amp;COUNTIF($L$1:L13,L13)</f>
+      <c r="AQ13" s="14" t="str">
+        <f>R13&amp;"-"&amp;COUNTIF($R$1:R13,R13)</f>
         <v>ESTADOS UNIDOS - Persona Física-9</v>
       </c>
-      <c r="AN13" s="1">
+      <c r="AR13" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO13" s="1">
+      <c r="AS13" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP13" s="1" t="str">
+      <c r="AT13" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ13" s="1">
+      <c r="AU13" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS13" s="2"/>
-      <c r="AT13" s="2"/>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="7">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C14" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I14" s="24" t="s">
         <v>1233</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M14" s="23">
-        <f>IFERROR(VLOOKUP(L14,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S14" s="23">
+        <f>IFERROR(VLOOKUP(R14,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2" t="s">
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S14" s="6" t="s">
+      <c r="Y14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="T14" s="4">
+      <c r="Z14" s="4">
         <v>7.0247929999999998</v>
       </c>
-      <c r="U14" s="5">
+      <c r="AA14" s="5">
         <v>19000</v>
       </c>
-      <c r="V14" s="5">
+      <c r="AB14" s="5">
         <f t="shared" si="10"/>
         <v>133471.06700000001</v>
       </c>
-      <c r="W14" s="10" t="s">
+      <c r="AC14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="X14" s="10" t="s">
+      <c r="AD14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Y14" s="10" t="s">
+      <c r="AE14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Z14" s="11">
+      <c r="AF14" s="11">
         <v>44816</v>
       </c>
-      <c r="AA14" s="13">
-        <f>COUNTIFS($D$1:D14,D14,$O$1:O14,O14)+1</f>
+      <c r="AG14" s="13">
+        <f>COUNTIFS($J$1:J14,J14,$U$1:U14,U14)+1</f>
         <v>2</v>
       </c>
-      <c r="AB14" s="15" t="str">
+      <c r="AH14" s="15" t="str">
         <f t="shared" si="11"/>
         <v>7.024793</v>
       </c>
-      <c r="AC14" s="15" t="str">
+      <c r="AI14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD14" s="1" t="str">
+      <c r="AJ14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="AE14" s="1" t="str">
+      <c r="AK14" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000150</v>
       </c>
-      <c r="AF14" s="8">
+      <c r="AL14" s="8">
         <f t="shared" si="12"/>
         <v>44816</v>
       </c>
-      <c r="AG14" s="12">
-        <f>IF(AP14="A",ROUND(V14+#REF!,2),ROUND(V14,2))</f>
+      <c r="AM14" s="12">
+        <f>IF(AT14="A",ROUND(AB14+#REF!,2),ROUND(AB14,2))</f>
         <v>133471.07</v>
       </c>
-      <c r="AH14" s="9" t="str">
+      <c r="AN14" s="9" t="str">
         <f t="shared" si="3"/>
         <v>133471.07</v>
       </c>
-      <c r="AI14" s="9" t="str">
+      <c r="AO14" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.93</v>
       </c>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="1">
+      <c r="AP14" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="AM14" s="14" t="str">
-        <f>L14&amp;"-"&amp;COUNTIF($L$1:L14,L14)</f>
+      <c r="AQ14" s="14" t="str">
+        <f>R14&amp;"-"&amp;COUNTIF($R$1:R14,R14)</f>
         <v>ESTADOS UNIDOS - Persona Física-10</v>
       </c>
-      <c r="AN14" s="1">
+      <c r="AR14" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO14" s="1">
+      <c r="AS14" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP14" s="1" t="str">
+      <c r="AT14" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ14" s="1">
+      <c r="AU14" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="2"/>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="7">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C15" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I15" s="24" t="s">
         <v>1233</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M15" s="23">
-        <f>IFERROR(VLOOKUP(L15,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S15" s="23">
+        <f>IFERROR(VLOOKUP(R15,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2" t="s">
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S15" s="6" t="s">
+      <c r="Y15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="T15" s="4">
+      <c r="Z15" s="4">
         <v>1.5</v>
       </c>
-      <c r="U15" s="5">
+      <c r="AA15" s="5">
         <v>19000</v>
       </c>
-      <c r="V15" s="5">
+      <c r="AB15" s="5">
         <f t="shared" si="10"/>
         <v>28500</v>
       </c>
-      <c r="W15" s="10" t="s">
+      <c r="AC15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="X15" s="10" t="s">
+      <c r="AD15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Y15" s="10" t="s">
+      <c r="AE15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="Z15" s="11">
+      <c r="AF15" s="11">
         <v>44816</v>
       </c>
-      <c r="AA15" s="13">
-        <f>COUNTIFS($D$1:D15,D15,$O$1:O15,O15)+1</f>
+      <c r="AG15" s="13">
+        <f>COUNTIFS($J$1:J15,J15,$U$1:U15,U15)+1</f>
         <v>3</v>
       </c>
-      <c r="AB15" s="15" t="str">
+      <c r="AH15" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
-      <c r="AC15" s="15" t="str">
+      <c r="AI15" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD15" s="1" t="str">
+      <c r="AJ15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="AE15" s="1" t="str">
+      <c r="AK15" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000152</v>
       </c>
-      <c r="AF15" s="8">
+      <c r="AL15" s="8">
         <f t="shared" si="12"/>
         <v>44816</v>
       </c>
-      <c r="AG15" s="12">
-        <f>IF(AP15="A",ROUND(V15+#REF!,2),ROUND(V15,2))</f>
+      <c r="AM15" s="12">
+        <f>IF(AT15="A",ROUND(AB15+#REF!,2),ROUND(AB15,2))</f>
         <v>28500</v>
       </c>
-      <c r="AH15" s="9" t="str">
+      <c r="AN15" s="9" t="str">
         <f t="shared" si="3"/>
         <v>28500.00</v>
       </c>
-      <c r="AI15" s="9" t="str">
+      <c r="AO15" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.00</v>
       </c>
-      <c r="AJ15" s="2"/>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="1">
+      <c r="AP15" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="AM15" s="14" t="str">
-        <f>L15&amp;"-"&amp;COUNTIF($L$1:L15,L15)</f>
+      <c r="AQ15" s="14" t="str">
+        <f>R15&amp;"-"&amp;COUNTIF($R$1:R15,R15)</f>
         <v>ESTADOS UNIDOS - Persona Física-11</v>
       </c>
-      <c r="AN15" s="1">
+      <c r="AR15" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO15" s="1">
+      <c r="AS15" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP15" s="1" t="str">
+      <c r="AT15" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ15" s="1">
+      <c r="AU15" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS15" s="2"/>
-      <c r="AT15" s="2"/>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="7">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C16" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I16" s="24" t="s">
         <v>1233</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M16" s="23">
-        <f>IFERROR(VLOOKUP(L16,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S16" s="23">
+        <f>IFERROR(VLOOKUP(R16,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2" t="s">
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S16" s="6" t="s">
+      <c r="Y16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="4">
+      <c r="Z16" s="4">
         <v>7.003044</v>
       </c>
-      <c r="U16" s="5">
+      <c r="AA16" s="5">
         <v>19000</v>
       </c>
-      <c r="V16" s="5">
+      <c r="AB16" s="5">
         <f t="shared" si="10"/>
         <v>133057.83600000001</v>
       </c>
-      <c r="W16" s="10" t="s">
+      <c r="AC16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="X16" s="10" t="s">
+      <c r="AD16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Y16" s="10" t="s">
+      <c r="AE16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="Z16" s="11">
+      <c r="AF16" s="11">
         <v>44816</v>
       </c>
-      <c r="AA16" s="13">
-        <f>COUNTIFS($D$1:D16,D16,$O$1:O16,O16)+1</f>
+      <c r="AG16" s="13">
+        <f>COUNTIFS($J$1:J16,J16,$U$1:U16,U16)+1</f>
         <v>4</v>
       </c>
-      <c r="AB16" s="15" t="str">
+      <c r="AH16" s="15" t="str">
         <f t="shared" si="11"/>
         <v>7.003044</v>
       </c>
-      <c r="AC16" s="15" t="str">
+      <c r="AI16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD16" s="1" t="str">
+      <c r="AJ16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="AE16" s="1" t="str">
+      <c r="AK16" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000151</v>
       </c>
-      <c r="AF16" s="8">
+      <c r="AL16" s="8">
         <f t="shared" si="12"/>
         <v>44816</v>
       </c>
-      <c r="AG16" s="12">
-        <f>IF(AP16="A",ROUND(V16+#REF!,2),ROUND(V16,2))</f>
+      <c r="AM16" s="12">
+        <f>IF(AT16="A",ROUND(AB16+#REF!,2),ROUND(AB16,2))</f>
         <v>133057.84</v>
       </c>
-      <c r="AH16" s="9" t="str">
+      <c r="AN16" s="9" t="str">
         <f t="shared" si="3"/>
         <v>133057.84</v>
       </c>
-      <c r="AI16" s="9" t="str">
+      <c r="AO16" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.16</v>
       </c>
-      <c r="AJ16" s="2"/>
-      <c r="AK16" s="2"/>
-      <c r="AL16" s="1">
+      <c r="AP16" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="AM16" s="14" t="str">
-        <f>L16&amp;"-"&amp;COUNTIF($L$1:L16,L16)</f>
+      <c r="AQ16" s="14" t="str">
+        <f>R16&amp;"-"&amp;COUNTIF($R$1:R16,R16)</f>
         <v>ESTADOS UNIDOS - Persona Física-12</v>
       </c>
-      <c r="AN16" s="1">
+      <c r="AR16" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="1">
+      <c r="AS16" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AP16" s="1" t="str">
+      <c r="AT16" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ16" s="1">
+      <c r="AU16" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AS16" s="2"/>
-      <c r="AT16" s="2"/>
-    </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="7">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>45143</v>
-      </c>
-      <c r="C17" s="24" t="s">
+        <v>45200</v>
+      </c>
+      <c r="I17" s="24" t="s">
         <v>1233</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="M17" s="23">
-        <f>IFERROR(VLOOKUP(L17,CUIT_paises[],2,0),"")</f>
-        <v>50000002124</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S17" s="23">
+        <f>IFERROR(VLOOKUP(R17,CUIT_paises[],2,0),"")</f>
+        <v>50000002124</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2" t="s">
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="Y17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="T17" s="4">
+      <c r="Z17" s="4">
         <v>1.5</v>
       </c>
-      <c r="U17" s="5">
+      <c r="AA17" s="5">
         <v>19000</v>
       </c>
-      <c r="V17" s="5">
+      <c r="AB17" s="5">
         <f t="shared" si="10"/>
         <v>28500</v>
       </c>
-      <c r="W17" s="10" t="s">
+      <c r="AC17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X17" s="10" t="s">
+      <c r="AD17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Y17" s="10" t="s">
+      <c r="AE17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Z17" s="11">
+      <c r="AF17" s="11">
         <v>44816</v>
       </c>
-      <c r="AA17" s="13">
-        <f>COUNTIFS($D$1:D17,D17,$O$1:O17,O17)+1</f>
+      <c r="AG17" s="13">
+        <f>COUNTIFS($J$1:J17,J17,$U$1:U17,U17)+1</f>
         <v>5</v>
       </c>
-      <c r="AB17" s="15" t="str">
+      <c r="AH17" s="15" t="str">
         <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
-      <c r="AC17" s="15" t="str">
+      <c r="AI17" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19000.00</v>
       </c>
-      <c r="AD17" s="1" t="str">
+      <c r="AJ17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00002</v>
       </c>
-      <c r="AE17" s="1" t="str">
+      <c r="AK17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>00000153</v>
       </c>
-      <c r="AF17" s="8">
+      <c r="AL17" s="8">
         <f t="shared" si="12"/>
         <v>44816</v>
       </c>
-      <c r="AG17" s="12">
-        <f>IF(AP17="A",ROUND(V17+#REF!,2),ROUND(V17,2))</f>
+      <c r="AM17" s="12">
+        <f>IF(AT17="A",ROUND(AB17+#REF!,2),ROUND(AB17,2))</f>
         <v>28500</v>
       </c>
-      <c r="AH17" s="9" t="str">
+      <c r="AN17" s="9" t="str">
         <f t="shared" si="3"/>
         <v>28500.00</v>
       </c>
-      <c r="AI17" s="9" t="str">
+      <c r="AO17" s="9" t="str">
         <f t="shared" si="13"/>
         <v>0.00</v>
       </c>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
-      <c r="AL17" s="1">
+      <c r="AP17" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="AM17" s="14" t="str">
-        <f>L17&amp;"-"&amp;COUNTIF($L$1:L17,L17)</f>
+      <c r="AQ17" s="14" t="str">
+        <f>R17&amp;"-"&amp;COUNTIF($R$1:R17,R17)</f>
         <v>ESTADOS UNIDOS - Persona Física-13</v>
       </c>
-      <c r="AN17" s="1">
+      <c r="AR17" s="1">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AO17" s="1">
+      <c r="AS17" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP17" s="1" t="str">
+      <c r="AT17" s="1" t="str">
         <f t="shared" si="7"/>
         <v>E</v>
       </c>
-      <c r="AQ17" s="1">
+      <c r="AU17" s="1">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AR17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS17" s="2"/>
-      <c r="AT17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AT17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:AQ17">
-    <sortCondition ref="D2:D17"/>
-    <sortCondition ref="F2:F17"/>
+  <autoFilter ref="A1:AU1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:AU17">
+    <sortCondition ref="J2:J17"/>
     <sortCondition ref="L2:L17"/>
+    <sortCondition ref="R2:R17"/>
   </sortState>
-  <conditionalFormatting sqref="H2:H17">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>E2=" Servicios"</formula>
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>A2="SI"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS17">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AR2="SI"</formula>
+  <conditionalFormatting sqref="N2:N17">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>K2=" Servicios"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2:AR17 F2:G17" xr:uid="{ED506666-DA8E-4EA2-B12C-A79BFB246358}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A17 L2:M17 E2:E17" xr:uid="{ED506666-DA8E-4EA2-B12C-A79BFB246358}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7102,37 +7155,37 @@
           <x14:formula1>
             <xm:f>Tablas!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D17</xm:sqref>
+          <xm:sqref>J2:J17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBDEC88A-D78E-4FDE-870B-E7BE28CEAC1B}">
           <x14:formula1>
             <xm:f>Tablas!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E17</xm:sqref>
+          <xm:sqref>K2:K17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3E04EB0C-23E0-4624-9E51-E89CD9E12C7E}">
           <x14:formula1>
             <xm:f>Tablas!$E$2:$E$305</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K17</xm:sqref>
+          <xm:sqref>Q2:Q17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5B30DA9-FA89-4BFD-8DAC-2E0694906006}">
           <x14:formula1>
             <xm:f>Tablas!$G$2:$G$50</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I17</xm:sqref>
+          <xm:sqref>O2:O17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E2621F0F-D555-4484-8C91-C051139517F3}">
           <x14:formula1>
             <xm:f>Tablas!$I$2:$I$784</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L17</xm:sqref>
+          <xm:sqref>R2:R17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54F47ECB-E9CC-4D44-947C-7D4263625D83}">
           <x14:formula1>
             <xm:f>Tablas!$L$2:$L$12</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R17</xm:sqref>
+          <xm:sqref>X2:X17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>